<commit_message>
Update 1.5.7: Bug fixes and QoL
</commit_message>
<xml_diff>
--- a/pkg/excels/templates/Шаблон для импорта МЖД.xlsx
+++ b/pkg/excels/templates/Шаблон для импорта МЖД.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mamad\OneDrive\Desktop\ТГЭМ\backend-v2\pkg\excels\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA1564A-7B0C-4C47-AECD-338D1AF1C2A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3F098F-03FC-48DC-8F4A-19D2E9B3BEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="МЖД" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,21 @@
     <sheet name="Бригады" sheetId="3" r:id="rId4"/>
     <sheet name="Супервайзеры" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -517,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,7 +724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097094F9-7E6F-44E4-B859-0524084CD09F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>